<commit_message>
adding dist category and version type to excel
</commit_message>
<xml_diff>
--- a/edi/template.xlsx
+++ b/edi/template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t xml:space="preserve">Work ID</t>
   </si>
@@ -39,6 +39,12 @@
   </si>
   <si>
     <t xml:space="preserve">Language Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distribution Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version Type</t>
   </si>
   <si>
     <t xml:space="preserve">Alternate Titles</t>
@@ -246,7 +252,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -257,11 +263,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="33.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="58.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="33.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="49.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="15.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="58.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="33.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="49.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="15.31"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -295,8 +303,12 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="ALZ1" s="0"/>
-      <c r="AMA1" s="0"/>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="AMB1" s="0"/>
       <c r="AMC1" s="0"/>
       <c r="AMD1" s="0"/>
@@ -356,22 +368,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>

</xml_diff>

<commit_message>
added ownership shares to Excel
</commit_message>
<xml_diff>
--- a/edi/template.xlsx
+++ b/edi/template.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Works" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Recordings" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="R1C1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -56,7 +56,7 @@
     <t xml:space="preserve">Artists</t>
   </si>
   <si>
-    <t xml:space="preserve">Original Publishers: Name [IPI name#] Controlled</t>
+    <t xml:space="preserve">Original Publishers: Name [IPI name#] (Role) {PR,MR,SR} Controlled</t>
   </si>
   <si>
     <t xml:space="preserve">ISRC</t>
@@ -169,12 +169,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -240,7 +240,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFE5CA"/>
     <pageSetUpPr fitToPage="false"/>
@@ -248,28 +248,26 @@
   <dimension ref="A1:AMJ1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.31640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="33.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="58.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="33.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="49.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="15.31"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -331,7 +329,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFBCE4E5"/>
     <pageSetUpPr fitToPage="false"/>
@@ -346,18 +344,16 @@
       <selection pane="bottomRight" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.31640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="33.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="33.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="9" style="0" width="15.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>